<commit_message>
so läuft das py script richtig
</commit_message>
<xml_diff>
--- a/Data/ProbeDatenAnleitungDB05.xlsx
+++ b/Data/ProbeDatenAnleitungDB05.xlsx
@@ -8,20 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juliane.bonenkamp\HandArbeitenAnleitungenDB\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BE26B3-EB5A-4330-B98F-4D393D52D506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E26B327-80D7-48D4-B960-E5651305A35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{CC7E93E5-AD33-4D5D-8E04-BC231D993E75}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="2" xr2:uid="{CC7E93E5-AD33-4D5D-8E04-BC231D993E75}"/>
   </bookViews>
   <sheets>
     <sheet name="Vollständig" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
+    <sheet name="Kontrolle" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="209">
   <si>
     <t>MedienArt</t>
   </si>
@@ -389,9 +403,6 @@
     <t>Utensilo „To Go“</t>
   </si>
   <si>
-    <t>Jabanisch Quilten</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -558,6 +569,99 @@
   </si>
   <si>
     <t>XV</t>
+  </si>
+  <si>
+    <t>Japanisch Quilten</t>
+  </si>
+  <si>
+    <t>o.J.</t>
+  </si>
+  <si>
+    <t>AnzahlBuch</t>
+  </si>
+  <si>
+    <t>ZeitschriftenGesamt</t>
+  </si>
+  <si>
+    <t>Datenebank</t>
+  </si>
+  <si>
+    <t>1. Durchlauf</t>
+  </si>
+  <si>
+    <t>anleitung</t>
+  </si>
+  <si>
+    <t>anleitungautor</t>
+  </si>
+  <si>
+    <t>autor</t>
+  </si>
+  <si>
+    <t>buch</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>mediumautor</t>
+  </si>
+  <si>
+    <t>zeitschrift</t>
+  </si>
+  <si>
+    <t>2. Duchlauf</t>
+  </si>
+  <si>
+    <t>Veränderung</t>
+  </si>
+  <si>
+    <t>doppelte DS</t>
+  </si>
+  <si>
+    <t>1 Khakifarbene Bundfaltenhose</t>
+  </si>
+  <si>
+    <t>2 Khakifarbene Bundfaltenhose</t>
+  </si>
+  <si>
+    <t>3 Khakifarbene Bundfaltenhose</t>
+  </si>
+  <si>
+    <t>4 Khakifarbene Bundfaltenhose</t>
+  </si>
+  <si>
+    <t>5 Khakifarbene Bundfaltenhose</t>
+  </si>
+  <si>
+    <t>6 Khakifarbene Bundfaltenhose</t>
+  </si>
+  <si>
+    <t>7 Khakifarbene Bundfaltenhose</t>
+  </si>
+  <si>
+    <t>8 Khakifarbene Bundfaltenhose</t>
+  </si>
+  <si>
+    <t>9 Khakifarbene Bundfaltenhose</t>
+  </si>
+  <si>
+    <t>10 Khakifarbene Bundfaltenhose</t>
+  </si>
+  <si>
+    <t>11 Khakifarbene Bundfaltenhose</t>
+  </si>
+  <si>
+    <t>12 Khakifarbene Bundfaltenhose</t>
+  </si>
+  <si>
+    <t>13 Khakifarbene Bundfaltenhose</t>
+  </si>
+  <si>
+    <t>14 Khakifarbene Bundfaltenhose</t>
+  </si>
+  <si>
+    <t>SummeDS</t>
   </si>
 </sst>
 </file>
@@ -652,7 +756,7 @@
       <name val="Liberation Sans"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -699,6 +803,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -748,10 +864,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Accent" xfId="2" xr:uid="{1C3C9374-E2EF-4DB6-8B8B-F8F759FFE405}"/>
@@ -1105,10 +1223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E6F388-6528-40D4-A910-773B4225880C}">
-  <dimension ref="A1:X78"/>
+  <dimension ref="A1:Z78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="J86" sqref="J86"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
@@ -1134,7 +1252,7 @@
     <col min="25" max="25" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>85</v>
       </c>
@@ -1163,7 +1281,7 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
@@ -1172,7 +1290,7 @@
         <v>9</v>
       </c>
       <c r="M1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N1" t="s">
         <v>10</v>
@@ -1202,13 +1320,13 @@
         <v>16</v>
       </c>
       <c r="W1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1216,7 +1334,10 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
+        <v>164</v>
+      </c>
+      <c r="D2" t="s">
+        <v>179</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
@@ -1231,7 +1352,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O2" t="s">
         <v>23</v>
@@ -1242,7 +1363,7 @@
       <c r="R2" t="s">
         <v>21</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="U2">
@@ -1257,8 +1378,15 @@
       <c r="X2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:24">
+      <c r="Y2" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z2">
+        <f>7+14-2</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1281,7 +1409,7 @@
         <v>41</v>
       </c>
       <c r="K3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O3" t="s">
         <v>42</v>
@@ -1289,7 +1417,7 @@
       <c r="P3" t="s">
         <v>43</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="4" t="s">
         <v>44</v>
       </c>
       <c r="U3">
@@ -1301,27 +1429,37 @@
       <c r="X3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="Y3" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z3">
+        <f>64-9</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" t="s">
         <v>97</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
+      <c r="D4" t="s">
+        <v>179</v>
+      </c>
       <c r="E4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N4" t="s">
         <v>26</v>
       </c>
       <c r="R4" t="s">
-        <v>136</v>
-      </c>
-      <c r="T4" t="s">
+        <v>135</v>
+      </c>
+      <c r="T4" s="4" t="s">
         <v>98</v>
       </c>
       <c r="U4">
@@ -1331,100 +1469,109 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:26">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>123</v>
+      </c>
+      <c r="D5" t="s">
+        <v>179</v>
       </c>
       <c r="K5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N5" t="s">
         <v>26</v>
       </c>
       <c r="O5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P5" t="s">
-        <v>138</v>
-      </c>
-      <c r="T5" t="s">
+        <v>137</v>
+      </c>
+      <c r="T5" s="4" t="s">
         <v>114</v>
       </c>
       <c r="U5">
         <v>73</v>
       </c>
       <c r="W5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>178</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
       <c r="C6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" t="s">
+        <v>179</v>
+      </c>
+      <c r="K6" t="s">
+        <v>163</v>
+      </c>
+      <c r="N6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" t="s">
+        <v>138</v>
+      </c>
+      <c r="P6" t="s">
+        <v>137</v>
+      </c>
+      <c r="T6" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="K6" t="s">
-        <v>164</v>
-      </c>
-      <c r="N6" t="s">
-        <v>26</v>
-      </c>
-      <c r="O6" t="s">
-        <v>139</v>
-      </c>
-      <c r="P6" t="s">
-        <v>138</v>
-      </c>
-      <c r="T6" t="s">
-        <v>125</v>
       </c>
       <c r="U6">
         <v>77</v>
       </c>
       <c r="W6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>178</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>124</v>
+        <v>123</v>
+      </c>
+      <c r="D7" t="s">
+        <v>179</v>
       </c>
       <c r="K7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N7" t="s">
         <v>26</v>
       </c>
       <c r="O7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P7" t="s">
-        <v>138</v>
-      </c>
-      <c r="T7" t="s">
-        <v>127</v>
+        <v>137</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="U7">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:26">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1447,7 +1594,7 @@
         <v>32</v>
       </c>
       <c r="K8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O8" t="s">
         <v>33</v>
@@ -1458,7 +1605,7 @@
       <c r="Q8" t="s">
         <v>35</v>
       </c>
-      <c r="T8" t="s">
+      <c r="T8" s="3" t="s">
         <v>61</v>
       </c>
       <c r="U8">
@@ -1471,7 +1618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:26">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1490,7 +1637,7 @@
       <c r="R9" t="s">
         <v>48</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9" s="3" t="s">
         <v>49</v>
       </c>
       <c r="U9">
@@ -1503,9 +1650,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:26">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
         <v>47</v>
@@ -1523,8 +1670,8 @@
       <c r="R10" t="s">
         <v>48</v>
       </c>
-      <c r="T10" t="s">
-        <v>128</v>
+      <c r="T10" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="U10">
         <v>25</v>
@@ -1533,7 +1680,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:26">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1555,7 +1702,7 @@
       <c r="R11" t="s">
         <v>55</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11" s="3" t="s">
         <v>56</v>
       </c>
       <c r="U11">
@@ -1568,7 +1715,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:26">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -1582,7 +1729,7 @@
         <v>2018</v>
       </c>
       <c r="M12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N12" t="s">
         <v>26</v>
@@ -1590,14 +1737,14 @@
       <c r="R12" t="s">
         <v>55</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T12" s="3" t="s">
         <v>114</v>
       </c>
       <c r="U12">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:26">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1616,7 +1763,7 @@
       <c r="R13" t="s">
         <v>51</v>
       </c>
-      <c r="T13" t="s">
+      <c r="T13" s="3" t="s">
         <v>52</v>
       </c>
       <c r="U13">
@@ -1626,7 +1773,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:26">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -1648,7 +1795,7 @@
       <c r="R14" t="s">
         <v>59</v>
       </c>
-      <c r="T14" t="s">
+      <c r="T14" s="3" t="s">
         <v>68</v>
       </c>
       <c r="U14">
@@ -1658,7 +1805,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:26">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -1680,7 +1827,7 @@
       <c r="R15" t="s">
         <v>87</v>
       </c>
-      <c r="T15" t="s">
+      <c r="T15" s="3" t="s">
         <v>70</v>
       </c>
       <c r="U15">
@@ -1693,7 +1840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:26">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1715,7 +1862,7 @@
       <c r="R16" t="s">
         <v>87</v>
       </c>
-      <c r="T16" t="s">
+      <c r="T16" s="3" t="s">
         <v>71</v>
       </c>
       <c r="U16">
@@ -1750,7 +1897,7 @@
       <c r="R17" t="s">
         <v>87</v>
       </c>
-      <c r="T17" t="s">
+      <c r="T17" s="3" t="s">
         <v>72</v>
       </c>
       <c r="U17">
@@ -1785,7 +1932,7 @@
       <c r="R18" t="s">
         <v>87</v>
       </c>
-      <c r="T18" t="s">
+      <c r="T18" s="3" t="s">
         <v>73</v>
       </c>
       <c r="U18">
@@ -1820,7 +1967,7 @@
       <c r="R19" t="s">
         <v>87</v>
       </c>
-      <c r="T19" t="s">
+      <c r="T19" s="3" t="s">
         <v>81</v>
       </c>
       <c r="U19">
@@ -1843,6 +1990,9 @@
       <c r="J20" t="s">
         <v>69</v>
       </c>
+      <c r="K20" t="s">
+        <v>163</v>
+      </c>
       <c r="M20">
         <v>43</v>
       </c>
@@ -1852,7 +2002,7 @@
       <c r="R20" t="s">
         <v>87</v>
       </c>
-      <c r="T20" t="s">
+      <c r="T20" s="3" t="s">
         <v>104</v>
       </c>
       <c r="U20">
@@ -1885,7 +2035,7 @@
       <c r="R21" t="s">
         <v>87</v>
       </c>
-      <c r="T21" t="s">
+      <c r="T21" s="3" t="s">
         <v>111</v>
       </c>
       <c r="U21">
@@ -1894,13 +2044,13 @@
     </row>
     <row r="22" spans="1:23">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B22" t="s">
         <v>47</v>
       </c>
       <c r="K22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -1909,10 +2059,10 @@
         <v>26</v>
       </c>
       <c r="R22" t="s">
-        <v>137</v>
-      </c>
-      <c r="T22" t="s">
-        <v>130</v>
+        <v>136</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="U22">
         <v>62</v>
@@ -1920,13 +2070,13 @@
     </row>
     <row r="23" spans="1:23">
       <c r="A23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B23" t="s">
         <v>47</v>
       </c>
       <c r="K23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -1935,10 +2085,10 @@
         <v>26</v>
       </c>
       <c r="R23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="T23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="U23">
         <v>64</v>
@@ -1946,13 +2096,13 @@
     </row>
     <row r="24" spans="1:23">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B24" t="s">
         <v>47</v>
       </c>
       <c r="K24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -1961,10 +2111,10 @@
         <v>26</v>
       </c>
       <c r="R24" t="s">
-        <v>137</v>
-      </c>
-      <c r="T24" t="s">
-        <v>131</v>
+        <v>136</v>
+      </c>
+      <c r="T24" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="U24">
         <v>64</v>
@@ -2024,7 +2174,7 @@
       <c r="R26" t="s">
         <v>88</v>
       </c>
-      <c r="T26" t="s">
+      <c r="T26" s="3" t="s">
         <v>78</v>
       </c>
       <c r="U26">
@@ -2056,7 +2206,7 @@
       <c r="R27" t="s">
         <v>88</v>
       </c>
-      <c r="T27" t="s">
+      <c r="T27" s="3" t="s">
         <v>79</v>
       </c>
       <c r="U27">
@@ -2089,7 +2239,7 @@
       <c r="R28" t="s">
         <v>88</v>
       </c>
-      <c r="T28" t="s">
+      <c r="T28" s="3" t="s">
         <v>95</v>
       </c>
       <c r="U28">
@@ -2149,7 +2299,7 @@
       <c r="R30" t="s">
         <v>88</v>
       </c>
-      <c r="T30" t="s">
+      <c r="T30" s="3" t="s">
         <v>95</v>
       </c>
       <c r="U30">
@@ -2179,7 +2329,7 @@
       <c r="R31" t="s">
         <v>88</v>
       </c>
-      <c r="T31" t="s">
+      <c r="T31" s="3" t="s">
         <v>96</v>
       </c>
       <c r="U31">
@@ -2208,7 +2358,7 @@
       <c r="R32" t="s">
         <v>88</v>
       </c>
-      <c r="T32" t="s">
+      <c r="T32" s="3" t="s">
         <v>84</v>
       </c>
       <c r="U32">
@@ -2241,7 +2391,7 @@
       <c r="R33" t="s">
         <v>88</v>
       </c>
-      <c r="T33" t="s">
+      <c r="T33" s="3" t="s">
         <v>100</v>
       </c>
       <c r="U33">
@@ -2271,7 +2421,7 @@
       <c r="R34" t="s">
         <v>88</v>
       </c>
-      <c r="T34" t="s">
+      <c r="T34" s="3" t="s">
         <v>101</v>
       </c>
       <c r="U34">
@@ -2331,7 +2481,7 @@
       <c r="R36" t="s">
         <v>88</v>
       </c>
-      <c r="T36" t="s">
+      <c r="T36" s="3" t="s">
         <v>115</v>
       </c>
       <c r="U36">
@@ -2391,7 +2541,7 @@
       <c r="R38" t="s">
         <v>88</v>
       </c>
-      <c r="T38" t="s">
+      <c r="T38" s="3" t="s">
         <v>116</v>
       </c>
       <c r="U38">
@@ -2421,7 +2571,7 @@
       <c r="R39" t="s">
         <v>88</v>
       </c>
-      <c r="T39" t="s">
+      <c r="T39" s="3" t="s">
         <v>116</v>
       </c>
       <c r="U39">
@@ -2541,7 +2691,7 @@
       <c r="R43" t="s">
         <v>88</v>
       </c>
-      <c r="T43" t="s">
+      <c r="T43" s="3" t="s">
         <v>117</v>
       </c>
       <c r="U43">
@@ -2571,7 +2721,7 @@
       <c r="R44" t="s">
         <v>88</v>
       </c>
-      <c r="T44" t="s">
+      <c r="T44" s="3" t="s">
         <v>118</v>
       </c>
       <c r="U44">
@@ -2601,7 +2751,7 @@
       <c r="R45" t="s">
         <v>88</v>
       </c>
-      <c r="T45" t="s">
+      <c r="T45" s="3" t="s">
         <v>119</v>
       </c>
       <c r="U45">
@@ -2631,7 +2781,7 @@
       <c r="R46" t="s">
         <v>88</v>
       </c>
-      <c r="T46" t="s">
+      <c r="T46" s="3" t="s">
         <v>120</v>
       </c>
       <c r="U46">
@@ -2660,7 +2810,7 @@
       <c r="R47" t="s">
         <v>59</v>
       </c>
-      <c r="T47" t="s">
+      <c r="T47" s="3" t="s">
         <v>60</v>
       </c>
       <c r="U47">
@@ -2717,7 +2867,7 @@
       <c r="R49" t="s">
         <v>59</v>
       </c>
-      <c r="T49" t="s">
+      <c r="T49" s="3" t="s">
         <v>90</v>
       </c>
       <c r="U49">
@@ -2747,7 +2897,7 @@
       <c r="R50" t="s">
         <v>59</v>
       </c>
-      <c r="T50" t="s">
+      <c r="T50" s="3" t="s">
         <v>102</v>
       </c>
       <c r="U50">
@@ -2774,7 +2924,7 @@
       <c r="R51" t="s">
         <v>59</v>
       </c>
-      <c r="T51" t="s">
+      <c r="T51" s="3" t="s">
         <v>121</v>
       </c>
       <c r="U51">
@@ -2803,7 +2953,7 @@
       <c r="R52" t="s">
         <v>59</v>
       </c>
-      <c r="T52" t="s">
+      <c r="T52" s="3" t="s">
         <v>64</v>
       </c>
       <c r="U52">
@@ -2835,7 +2985,7 @@
       <c r="R53" t="s">
         <v>59</v>
       </c>
-      <c r="T53" t="s">
+      <c r="T53" s="3" t="s">
         <v>74</v>
       </c>
       <c r="U53">
@@ -2867,7 +3017,7 @@
       <c r="R54" t="s">
         <v>59</v>
       </c>
-      <c r="T54" t="s">
+      <c r="T54" s="3" t="s">
         <v>75</v>
       </c>
       <c r="U54">
@@ -2899,7 +3049,7 @@
       <c r="R55" t="s">
         <v>59</v>
       </c>
-      <c r="T55" t="s">
+      <c r="T55" s="3" t="s">
         <v>80</v>
       </c>
       <c r="U55">
@@ -2930,9 +3080,9 @@
         <v>26</v>
       </c>
       <c r="R56" t="s">
-        <v>137</v>
-      </c>
-      <c r="T56" t="s">
+        <v>136</v>
+      </c>
+      <c r="T56" s="3" t="s">
         <v>103</v>
       </c>
       <c r="U56">
@@ -2960,9 +3110,9 @@
         <v>26</v>
       </c>
       <c r="R57" t="s">
-        <v>137</v>
-      </c>
-      <c r="T57" t="s">
+        <v>136</v>
+      </c>
+      <c r="T57" s="3" t="s">
         <v>103</v>
       </c>
       <c r="U57">
@@ -2990,9 +3140,9 @@
         <v>26</v>
       </c>
       <c r="R58" t="s">
-        <v>137</v>
-      </c>
-      <c r="T58" t="s">
+        <v>136</v>
+      </c>
+      <c r="T58" s="3" t="s">
         <v>105</v>
       </c>
       <c r="U58">
@@ -3020,9 +3170,9 @@
         <v>26</v>
       </c>
       <c r="R59" t="s">
-        <v>137</v>
-      </c>
-      <c r="T59" t="s">
+        <v>136</v>
+      </c>
+      <c r="T59" s="3" t="s">
         <v>108</v>
       </c>
       <c r="U59">
@@ -3050,9 +3200,9 @@
         <v>26</v>
       </c>
       <c r="R60" t="s">
-        <v>137</v>
-      </c>
-      <c r="T60" t="s">
+        <v>136</v>
+      </c>
+      <c r="T60" s="3" t="s">
         <v>109</v>
       </c>
       <c r="U60">
@@ -3080,9 +3230,9 @@
         <v>26</v>
       </c>
       <c r="R61" t="s">
-        <v>137</v>
-      </c>
-      <c r="T61" t="s">
+        <v>136</v>
+      </c>
+      <c r="T61" s="3" t="s">
         <v>110</v>
       </c>
       <c r="U61">
@@ -3100,7 +3250,7 @@
         <v>92</v>
       </c>
       <c r="K62" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M62" t="s">
         <v>93</v>
@@ -3109,9 +3259,9 @@
         <v>36</v>
       </c>
       <c r="R62" t="s">
-        <v>137</v>
-      </c>
-      <c r="T62" t="s">
+        <v>136</v>
+      </c>
+      <c r="T62" s="3" t="s">
         <v>94</v>
       </c>
       <c r="U62">
@@ -3143,7 +3293,7 @@
       <c r="R63" t="s">
         <v>59</v>
       </c>
-      <c r="T63" t="s">
+      <c r="T63" s="3" t="s">
         <v>66</v>
       </c>
       <c r="U63">
@@ -3175,7 +3325,7 @@
       <c r="R64" t="s">
         <v>59</v>
       </c>
-      <c r="T64" t="s">
+      <c r="T64" s="3" t="s">
         <v>106</v>
       </c>
       <c r="U64">
@@ -3190,7 +3340,10 @@
         <v>19</v>
       </c>
       <c r="C65" t="s">
-        <v>166</v>
+        <v>165</v>
+      </c>
+      <c r="D65" t="s">
+        <v>179</v>
       </c>
       <c r="E65" t="s">
         <v>21</v>
@@ -3205,7 +3358,7 @@
         <v>2</v>
       </c>
       <c r="K65" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O65" t="s">
         <v>23</v>
@@ -3216,8 +3369,8 @@
       <c r="R65" t="s">
         <v>21</v>
       </c>
-      <c r="T65" t="s">
-        <v>25</v>
+      <c r="T65" s="4" t="s">
+        <v>194</v>
       </c>
       <c r="U65">
         <v>345</v>
@@ -3240,7 +3393,10 @@
         <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>167</v>
+        <v>166</v>
+      </c>
+      <c r="D66" t="s">
+        <v>179</v>
       </c>
       <c r="E66" t="s">
         <v>21</v>
@@ -3255,7 +3411,7 @@
         <v>3</v>
       </c>
       <c r="K66" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O66" t="s">
         <v>23</v>
@@ -3266,8 +3422,8 @@
       <c r="R66" t="s">
         <v>21</v>
       </c>
-      <c r="T66" t="s">
-        <v>25</v>
+      <c r="T66" s="4" t="s">
+        <v>195</v>
       </c>
       <c r="U66">
         <v>355</v>
@@ -3290,7 +3446,10 @@
         <v>19</v>
       </c>
       <c r="C67" t="s">
-        <v>168</v>
+        <v>167</v>
+      </c>
+      <c r="D67" t="s">
+        <v>179</v>
       </c>
       <c r="E67" t="s">
         <v>21</v>
@@ -3305,7 +3464,7 @@
         <v>4</v>
       </c>
       <c r="K67" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O67" t="s">
         <v>23</v>
@@ -3316,8 +3475,8 @@
       <c r="R67" t="s">
         <v>21</v>
       </c>
-      <c r="T67" t="s">
-        <v>25</v>
+      <c r="T67" s="4" t="s">
+        <v>196</v>
       </c>
       <c r="U67">
         <v>365</v>
@@ -3340,7 +3499,10 @@
         <v>19</v>
       </c>
       <c r="C68" t="s">
-        <v>169</v>
+        <v>168</v>
+      </c>
+      <c r="D68" t="s">
+        <v>179</v>
       </c>
       <c r="E68" t="s">
         <v>21</v>
@@ -3355,7 +3517,7 @@
         <v>5</v>
       </c>
       <c r="K68" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O68" t="s">
         <v>23</v>
@@ -3366,8 +3528,8 @@
       <c r="R68" t="s">
         <v>21</v>
       </c>
-      <c r="T68" t="s">
-        <v>25</v>
+      <c r="T68" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="U68">
         <v>375</v>
@@ -3390,7 +3552,10 @@
         <v>19</v>
       </c>
       <c r="C69" t="s">
-        <v>170</v>
+        <v>169</v>
+      </c>
+      <c r="D69" t="s">
+        <v>179</v>
       </c>
       <c r="E69" t="s">
         <v>21</v>
@@ -3405,7 +3570,7 @@
         <v>6</v>
       </c>
       <c r="K69" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O69" t="s">
         <v>23</v>
@@ -3416,8 +3581,8 @@
       <c r="R69" t="s">
         <v>21</v>
       </c>
-      <c r="T69" t="s">
-        <v>25</v>
+      <c r="T69" s="4" t="s">
+        <v>198</v>
       </c>
       <c r="U69">
         <v>385</v>
@@ -3440,7 +3605,10 @@
         <v>19</v>
       </c>
       <c r="C70" t="s">
-        <v>171</v>
+        <v>170</v>
+      </c>
+      <c r="D70" t="s">
+        <v>179</v>
       </c>
       <c r="E70" t="s">
         <v>21</v>
@@ -3455,7 +3623,7 @@
         <v>7</v>
       </c>
       <c r="K70" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O70" t="s">
         <v>23</v>
@@ -3466,8 +3634,8 @@
       <c r="R70" t="s">
         <v>21</v>
       </c>
-      <c r="T70" t="s">
-        <v>25</v>
+      <c r="T70" s="4" t="s">
+        <v>199</v>
       </c>
       <c r="U70">
         <v>395</v>
@@ -3490,7 +3658,10 @@
         <v>19</v>
       </c>
       <c r="C71" t="s">
-        <v>172</v>
+        <v>171</v>
+      </c>
+      <c r="D71" t="s">
+        <v>179</v>
       </c>
       <c r="E71" t="s">
         <v>21</v>
@@ -3505,7 +3676,7 @@
         <v>8</v>
       </c>
       <c r="K71" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O71" t="s">
         <v>23</v>
@@ -3516,8 +3687,8 @@
       <c r="R71" t="s">
         <v>21</v>
       </c>
-      <c r="T71" t="s">
-        <v>25</v>
+      <c r="T71" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="U71">
         <v>405</v>
@@ -3540,7 +3711,10 @@
         <v>19</v>
       </c>
       <c r="C72" t="s">
-        <v>173</v>
+        <v>172</v>
+      </c>
+      <c r="D72" t="s">
+        <v>179</v>
       </c>
       <c r="E72" t="s">
         <v>21</v>
@@ -3555,7 +3729,7 @@
         <v>9</v>
       </c>
       <c r="K72" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O72" t="s">
         <v>23</v>
@@ -3566,8 +3740,8 @@
       <c r="R72" t="s">
         <v>21</v>
       </c>
-      <c r="T72" t="s">
-        <v>25</v>
+      <c r="T72" s="4" t="s">
+        <v>201</v>
       </c>
       <c r="U72">
         <v>415</v>
@@ -3592,6 +3766,9 @@
       <c r="C73" t="s">
         <v>20</v>
       </c>
+      <c r="D73" t="s">
+        <v>179</v>
+      </c>
       <c r="E73" t="s">
         <v>21</v>
       </c>
@@ -3605,7 +3782,7 @@
         <v>10</v>
       </c>
       <c r="K73" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O73" t="s">
         <v>23</v>
@@ -3616,8 +3793,8 @@
       <c r="R73" t="s">
         <v>21</v>
       </c>
-      <c r="T73" t="s">
-        <v>25</v>
+      <c r="T73" s="4" t="s">
+        <v>202</v>
       </c>
       <c r="U73">
         <v>425</v>
@@ -3640,7 +3817,10 @@
         <v>19</v>
       </c>
       <c r="C74" t="s">
-        <v>174</v>
+        <v>173</v>
+      </c>
+      <c r="D74" t="s">
+        <v>179</v>
       </c>
       <c r="E74" t="s">
         <v>21</v>
@@ -3655,7 +3835,7 @@
         <v>11</v>
       </c>
       <c r="K74" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O74" t="s">
         <v>23</v>
@@ -3666,8 +3846,8 @@
       <c r="R74" t="s">
         <v>21</v>
       </c>
-      <c r="T74" t="s">
-        <v>25</v>
+      <c r="T74" s="4" t="s">
+        <v>203</v>
       </c>
       <c r="U74">
         <v>435</v>
@@ -3690,7 +3870,10 @@
         <v>19</v>
       </c>
       <c r="C75" t="s">
-        <v>175</v>
+        <v>174</v>
+      </c>
+      <c r="D75" t="s">
+        <v>179</v>
       </c>
       <c r="E75" t="s">
         <v>21</v>
@@ -3705,7 +3888,7 @@
         <v>12</v>
       </c>
       <c r="K75" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O75" t="s">
         <v>23</v>
@@ -3716,8 +3899,8 @@
       <c r="R75" t="s">
         <v>21</v>
       </c>
-      <c r="T75" t="s">
-        <v>25</v>
+      <c r="T75" s="4" t="s">
+        <v>204</v>
       </c>
       <c r="U75">
         <v>445</v>
@@ -3740,7 +3923,10 @@
         <v>19</v>
       </c>
       <c r="C76" t="s">
-        <v>176</v>
+        <v>175</v>
+      </c>
+      <c r="D76" t="s">
+        <v>179</v>
       </c>
       <c r="E76" t="s">
         <v>21</v>
@@ -3755,7 +3941,7 @@
         <v>13</v>
       </c>
       <c r="K76" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O76" t="s">
         <v>23</v>
@@ -3766,8 +3952,8 @@
       <c r="R76" t="s">
         <v>21</v>
       </c>
-      <c r="T76" t="s">
-        <v>25</v>
+      <c r="T76" s="4" t="s">
+        <v>205</v>
       </c>
       <c r="U76">
         <v>455</v>
@@ -3790,7 +3976,10 @@
         <v>19</v>
       </c>
       <c r="C77" t="s">
-        <v>177</v>
+        <v>176</v>
+      </c>
+      <c r="D77" t="s">
+        <v>179</v>
       </c>
       <c r="E77" t="s">
         <v>21</v>
@@ -3805,7 +3994,7 @@
         <v>14</v>
       </c>
       <c r="K77" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O77" t="s">
         <v>23</v>
@@ -3816,8 +4005,8 @@
       <c r="R77" t="s">
         <v>21</v>
       </c>
-      <c r="T77" t="s">
-        <v>25</v>
+      <c r="T77" s="4" t="s">
+        <v>206</v>
       </c>
       <c r="U77">
         <v>465</v>
@@ -3840,7 +4029,10 @@
         <v>19</v>
       </c>
       <c r="C78" t="s">
-        <v>178</v>
+        <v>177</v>
+      </c>
+      <c r="D78" t="s">
+        <v>179</v>
       </c>
       <c r="E78" t="s">
         <v>21</v>
@@ -3855,7 +4047,7 @@
         <v>15</v>
       </c>
       <c r="K78" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O78" t="s">
         <v>23</v>
@@ -3866,8 +4058,8 @@
       <c r="R78" t="s">
         <v>21</v>
       </c>
-      <c r="T78" t="s">
-        <v>25</v>
+      <c r="T78" s="4" t="s">
+        <v>207</v>
       </c>
       <c r="U78">
         <v>475</v>
@@ -3937,7 +4129,7 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
@@ -3946,7 +4138,7 @@
         <v>9</v>
       </c>
       <c r="M1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N1" t="s">
         <v>10</v>
@@ -3976,42 +4168,42 @@
         <v>16</v>
       </c>
       <c r="W1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="X1" t="s">
         <v>17</v>
       </c>
       <c r="Y1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z1" t="s">
         <v>141</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>142</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>143</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>144</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>145</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:30">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
+        <v>149</v>
+      </c>
+      <c r="R2" t="s">
         <v>150</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>151</v>
-      </c>
-      <c r="T2" t="s">
-        <v>152</v>
       </c>
       <c r="U2">
         <v>5</v>
@@ -4020,13 +4212,13 @@
         <v>36</v>
       </c>
       <c r="Y2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="Z2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AA2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AB2">
         <v>2018</v>
@@ -4037,16 +4229,16 @@
     </row>
     <row r="3" spans="1:30">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R3" t="s">
+        <v>154</v>
+      </c>
+      <c r="T3" t="s">
         <v>155</v>
-      </c>
-      <c r="T3" t="s">
-        <v>156</v>
       </c>
       <c r="U3">
         <v>4</v>
@@ -4055,16 +4247,16 @@
         <v>26</v>
       </c>
       <c r="W3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Y3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AB3" s="2">
         <v>43809</v>
@@ -4075,13 +4267,13 @@
     </row>
     <row r="4" spans="1:30">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="T4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="U4">
         <v>7</v>
@@ -4090,22 +4282,383 @@
         <v>36</v>
       </c>
       <c r="W4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Y4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Z4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AA4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AB4" s="2">
         <v>43809</v>
       </c>
       <c r="AC4" t="s">
         <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5CA3F7-3463-4F3E-BB07-77B22D87594D}">
+  <dimension ref="A1:X12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H1" t="s">
+        <v>190</v>
+      </c>
+      <c r="I1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2">
+        <v>68</v>
+      </c>
+      <c r="C2">
+        <v>68</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>19</v>
+      </c>
+      <c r="F2">
+        <v>42</v>
+      </c>
+      <c r="G2">
+        <v>43</v>
+      </c>
+      <c r="H2">
+        <v>23</v>
+      </c>
+      <c r="I2">
+        <f>SUM(B2:H2)</f>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" hidden="1">
+      <c r="A3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3">
+        <v>116</v>
+      </c>
+      <c r="C3">
+        <v>116</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>44</v>
+      </c>
+      <c r="G3">
+        <v>53</v>
+      </c>
+      <c r="H3">
+        <v>24</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I6" si="0">SUM(B3:H3)</f>
+        <v>385</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" hidden="1">
+      <c r="B4">
+        <v>68</v>
+      </c>
+      <c r="C4">
+        <v>68</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>19</v>
+      </c>
+      <c r="F4">
+        <v>42</v>
+      </c>
+      <c r="G4">
+        <v>43</v>
+      </c>
+      <c r="H4">
+        <v>23</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="B5">
+        <v>115</v>
+      </c>
+      <c r="C5">
+        <v>115</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>19</v>
+      </c>
+      <c r="F5">
+        <v>42</v>
+      </c>
+      <c r="G5">
+        <v>50</v>
+      </c>
+      <c r="H5">
+        <v>23</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="B6">
+        <v>68</v>
+      </c>
+      <c r="C6">
+        <v>68</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>19</v>
+      </c>
+      <c r="F6">
+        <v>42</v>
+      </c>
+      <c r="G6">
+        <v>48</v>
+      </c>
+      <c r="H6">
+        <v>23</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="A7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7">
+        <f>B6-B2</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:H7" si="1">C6-C2</f>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="A9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" t="s">
+        <v>131</v>
+      </c>
+      <c r="K10" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" t="s">
+        <v>134</v>
+      </c>
+      <c r="N10" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" t="s">
+        <v>11</v>
+      </c>
+      <c r="P10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>13</v>
+      </c>
+      <c r="R10" t="s">
+        <v>14</v>
+      </c>
+      <c r="S10" t="s">
+        <v>15</v>
+      </c>
+      <c r="T10" t="s">
+        <v>86</v>
+      </c>
+      <c r="U10" t="s">
+        <v>89</v>
+      </c>
+      <c r="V10" t="s">
+        <v>16</v>
+      </c>
+      <c r="W10" t="s">
+        <v>133</v>
+      </c>
+      <c r="X10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="A11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E11" t="s">
+        <v>135</v>
+      </c>
+      <c r="K11" t="s">
+        <v>163</v>
+      </c>
+      <c r="N11" t="s">
+        <v>26</v>
+      </c>
+      <c r="R11" t="s">
+        <v>135</v>
+      </c>
+      <c r="T11" t="s">
+        <v>98</v>
+      </c>
+      <c r="U11">
+        <v>9</v>
+      </c>
+      <c r="W11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" t="s">
+        <v>163</v>
+      </c>
+      <c r="M12">
+        <v>43</v>
+      </c>
+      <c r="N12" t="s">
+        <v>26</v>
+      </c>
+      <c r="R12" t="s">
+        <v>87</v>
+      </c>
+      <c r="T12" t="s">
+        <v>104</v>
+      </c>
+      <c r="U12">
+        <v>26</v>
+      </c>
+      <c r="W12">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Vorbereitung für pdf als medium
</commit_message>
<xml_diff>
--- a/Data/ProbeDatenAnleitungDB05.xlsx
+++ b/Data/ProbeDatenAnleitungDB05.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juliane.bonenkamp\HandArbeitenAnleitungenDB\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E26B327-80D7-48D4-B960-E5651305A35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DD9AF1-B43B-40AD-9BED-602AD5F8E9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="2" xr2:uid="{CC7E93E5-AD33-4D5D-8E04-BC231D993E75}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{CC7E93E5-AD33-4D5D-8E04-BC231D993E75}"/>
   </bookViews>
   <sheets>
     <sheet name="Vollständig" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
+    <sheet name="ProbeDatenPDF" sheetId="2" r:id="rId2"/>
     <sheet name="Kontrolle" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -4090,7 +4090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5488032-BB51-4744-B401-BCB2F6646798}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
@@ -4309,7 +4309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5CA3F7-3463-4F3E-BB07-77B22D87594D}">
   <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Datein als neue MedienArt eingefügt
</commit_message>
<xml_diff>
--- a/Data/ProbeDatenAnleitungDB05.xlsx
+++ b/Data/ProbeDatenAnleitungDB05.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juliane.bonenkamp\HandArbeitenAnleitungenDB\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DD9AF1-B43B-40AD-9BED-602AD5F8E9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10523830-0F2F-406C-9930-F0F4914D25B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{CC7E93E5-AD33-4D5D-8E04-BC231D993E75}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="2" xr2:uid="{CC7E93E5-AD33-4D5D-8E04-BC231D993E75}"/>
   </bookViews>
   <sheets>
     <sheet name="Vollständig" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="211">
   <si>
     <t>MedienArt</t>
   </si>
@@ -454,9 +454,6 @@
     <t>Kutoh</t>
   </si>
   <si>
-    <t>C:\Users\juliane.bonenkamp\HandArbeitenAnleitungenDB\Data\strick\Mützen\1523941356_GestrickteTeufelsmtzeausRainbowBaumwolle.pdf</t>
-  </si>
-  <si>
     <t>Dateiname</t>
   </si>
   <si>
@@ -475,12 +472,6 @@
     <t>GanzerText</t>
   </si>
   <si>
-    <t>1523941356_GestrickteTeufelsmtzeausRainbowBaumwolle.pdf</t>
-  </si>
-  <si>
-    <t>1523941356_GestrickteTeufelsmtzeausRainbowBaumwolle</t>
-  </si>
-  <si>
     <t>pdf</t>
   </si>
   <si>
@@ -493,12 +484,6 @@
     <t>Gestrickte Teufelsmütze aus Rainbow Baumwolle</t>
   </si>
   <si>
-    <t>C:\Users\juliane.bonenkamp\HandArbeitenAnleitungenDB\Data\strick\Mützen\DROPS Extra 0-882 - Gestrickte DROPS Mütze mit Dominomuster aus _Delight_. - Free pattern by DROPS Design.pdf</t>
-  </si>
-  <si>
-    <t>DROPS Extra 0-882 - Gestrickte DROPS Mütze mit Dominomuster aus _Delight_. - Free pattern by DROPS Design.pdf</t>
-  </si>
-  <si>
     <t>Drops-Desing</t>
   </si>
   <si>
@@ -508,18 +493,6 @@
     <t>0-882</t>
   </si>
   <si>
-    <t>C:\Users\juliane.bonenkamp\HandArbeitenAnleitungenDB\Data\strick\Mützen\Granite - Gestrickte Mütze in DROPS Big Delight. Die Arbeit wird kraus rechts mit Pompon gestrickt. - Free pattern by DROPS Design.pdf</t>
-  </si>
-  <si>
-    <t>Granite - Gestrickte Mütze in DROPS Big Delight. Die Arbeit wird kraus rechts mit Pompon gestrickt. - Free pattern by DROPS Design.pdf</t>
-  </si>
-  <si>
-    <t>Granite - Gestrickte Mütze in DROPS Big Delight. Die Arbeit wird kraus rechts mit Pompon gestrickt</t>
-  </si>
-  <si>
-    <t>DROPS Extra 0-882 - Gestrickte DROPS Mütze mit Dominomuster aus _Delight</t>
-  </si>
-  <si>
     <t>Grante</t>
   </si>
   <si>
@@ -577,12 +550,6 @@
     <t>o.J.</t>
   </si>
   <si>
-    <t>AnzahlBuch</t>
-  </si>
-  <si>
-    <t>ZeitschriftenGesamt</t>
-  </si>
-  <si>
     <t>Datenebank</t>
   </si>
   <si>
@@ -662,6 +629,45 @@
   </si>
   <si>
     <t>SummeDS</t>
+  </si>
+  <si>
+    <t>C:\Users\juliane.bonenkamp\HandArbeitenAnleitungenDB\Data\strick\Mützen\GestrickteTeufelsmtzeRainbowBaumwolle.pdf</t>
+  </si>
+  <si>
+    <t>GestrickteTeufelsmtzeRainbowBaumwolle.pdf</t>
+  </si>
+  <si>
+    <t>GestrickteTeufelsmtzeRainbowBaumwolle</t>
+  </si>
+  <si>
+    <t>DROPSGestrickteMützeDominomuster.pdf</t>
+  </si>
+  <si>
+    <t>C:\Users\juliane.bonenkamp\HandArbeitenAnleitungenDB\Data\strick\Mützen\DROPSGestrickteMützeDominomuster.pdf</t>
+  </si>
+  <si>
+    <t>"C:\Users\juliane.bonenkamp\HandArbeitenAnleitungenDB\Data\strick\Mützen\Granite.pdf"</t>
+  </si>
+  <si>
+    <t>Granite.pdf</t>
+  </si>
+  <si>
+    <t>Granite</t>
+  </si>
+  <si>
+    <t>DROPSGestrickteMützeDominomuster</t>
+  </si>
+  <si>
+    <t>textdatei</t>
+  </si>
+  <si>
+    <t>Durchlauf</t>
+  </si>
+  <si>
+    <t>o.T.</t>
+  </si>
+  <si>
+    <t>Unvollsändiger Datensatz in der CSV</t>
   </si>
 </sst>
 </file>
@@ -1223,10 +1229,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E6F388-6528-40D4-A910-773B4225880C}">
-  <dimension ref="A1:Z78"/>
+  <dimension ref="A1:AD81"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
@@ -1252,7 +1258,7 @@
     <col min="25" max="25" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>85</v>
       </c>
@@ -1325,8 +1331,26 @@
       <c r="X1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:26">
+      <c r="Y1" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1334,10 +1358,10 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
@@ -1352,7 +1376,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O2" t="s">
         <v>23</v>
@@ -1378,15 +1402,8 @@
       <c r="X2" t="s">
         <v>27</v>
       </c>
-      <c r="Y2" t="s">
-        <v>180</v>
-      </c>
-      <c r="Z2">
-        <f>7+14-2</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26">
+    </row>
+    <row r="3" spans="1:30">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1409,7 +1426,7 @@
         <v>41</v>
       </c>
       <c r="K3" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O3" t="s">
         <v>42</v>
@@ -1429,29 +1446,25 @@
       <c r="X3" t="s">
         <v>45</v>
       </c>
-      <c r="Y3" t="s">
-        <v>181</v>
-      </c>
-      <c r="Z3">
-        <f>64-9</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26">
+    </row>
+    <row r="4" spans="1:30">
       <c r="A4" t="s">
         <v>97</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
+      <c r="C4" t="s">
+        <v>209</v>
+      </c>
       <c r="D4" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E4" t="s">
         <v>135</v>
       </c>
       <c r="K4" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="N4" t="s">
         <v>26</v>
@@ -1469,9 +1482,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:30">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -1480,10 +1493,10 @@
         <v>123</v>
       </c>
       <c r="D5" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="K5" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="N5" t="s">
         <v>26</v>
@@ -1504,9 +1517,9 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:30">
       <c r="A6" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -1515,10 +1528,10 @@
         <v>123</v>
       </c>
       <c r="D6" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="K6" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="N6" t="s">
         <v>26</v>
@@ -1539,9 +1552,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:30">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -1550,10 +1563,10 @@
         <v>123</v>
       </c>
       <c r="D7" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="K7" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="N7" t="s">
         <v>26</v>
@@ -1571,7 +1584,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:30">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1594,7 +1607,7 @@
         <v>32</v>
       </c>
       <c r="K8" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O8" t="s">
         <v>33</v>
@@ -1618,7 +1631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:30">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1650,7 +1663,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:30">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1680,7 +1693,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:30">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1715,7 +1728,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:30">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -1744,7 +1757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:30">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1773,7 +1786,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:30">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -1805,7 +1818,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:30">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -1840,7 +1853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:30">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1991,7 +2004,7 @@
         <v>69</v>
       </c>
       <c r="K20" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="M20">
         <v>43</v>
@@ -2050,7 +2063,7 @@
         <v>47</v>
       </c>
       <c r="K22" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -2076,7 +2089,7 @@
         <v>47</v>
       </c>
       <c r="K23" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -2102,7 +2115,7 @@
         <v>47</v>
       </c>
       <c r="K24" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -3250,7 +3263,7 @@
         <v>92</v>
       </c>
       <c r="K62" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="M62" t="s">
         <v>93</v>
@@ -3332,7 +3345,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:24">
+    <row r="65" spans="1:29">
       <c r="A65" t="s">
         <v>18</v>
       </c>
@@ -3340,10 +3353,10 @@
         <v>19</v>
       </c>
       <c r="C65" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="D65" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E65" t="s">
         <v>21</v>
@@ -3358,7 +3371,7 @@
         <v>2</v>
       </c>
       <c r="K65" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O65" t="s">
         <v>23</v>
@@ -3370,7 +3383,7 @@
         <v>21</v>
       </c>
       <c r="T65" s="4" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="U65">
         <v>345</v>
@@ -3385,7 +3398,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:24">
+    <row r="66" spans="1:29">
       <c r="A66" t="s">
         <v>18</v>
       </c>
@@ -3393,10 +3406,10 @@
         <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D66" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E66" t="s">
         <v>21</v>
@@ -3411,7 +3424,7 @@
         <v>3</v>
       </c>
       <c r="K66" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O66" t="s">
         <v>23</v>
@@ -3423,7 +3436,7 @@
         <v>21</v>
       </c>
       <c r="T66" s="4" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="U66">
         <v>355</v>
@@ -3438,7 +3451,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:24">
+    <row r="67" spans="1:29">
       <c r="A67" t="s">
         <v>18</v>
       </c>
@@ -3446,10 +3459,10 @@
         <v>19</v>
       </c>
       <c r="C67" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D67" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E67" t="s">
         <v>21</v>
@@ -3464,7 +3477,7 @@
         <v>4</v>
       </c>
       <c r="K67" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O67" t="s">
         <v>23</v>
@@ -3476,7 +3489,7 @@
         <v>21</v>
       </c>
       <c r="T67" s="4" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="U67">
         <v>365</v>
@@ -3491,7 +3504,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:24">
+    <row r="68" spans="1:29">
       <c r="A68" t="s">
         <v>18</v>
       </c>
@@ -3499,10 +3512,10 @@
         <v>19</v>
       </c>
       <c r="C68" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D68" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E68" t="s">
         <v>21</v>
@@ -3517,7 +3530,7 @@
         <v>5</v>
       </c>
       <c r="K68" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O68" t="s">
         <v>23</v>
@@ -3529,7 +3542,7 @@
         <v>21</v>
       </c>
       <c r="T68" s="4" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="U68">
         <v>375</v>
@@ -3544,7 +3557,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:24">
+    <row r="69" spans="1:29">
       <c r="A69" t="s">
         <v>18</v>
       </c>
@@ -3552,10 +3565,10 @@
         <v>19</v>
       </c>
       <c r="C69" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D69" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E69" t="s">
         <v>21</v>
@@ -3570,7 +3583,7 @@
         <v>6</v>
       </c>
       <c r="K69" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O69" t="s">
         <v>23</v>
@@ -3582,7 +3595,7 @@
         <v>21</v>
       </c>
       <c r="T69" s="4" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="U69">
         <v>385</v>
@@ -3597,7 +3610,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="70" spans="1:24">
+    <row r="70" spans="1:29">
       <c r="A70" t="s">
         <v>18</v>
       </c>
@@ -3605,10 +3618,10 @@
         <v>19</v>
       </c>
       <c r="C70" t="s">
+        <v>161</v>
+      </c>
+      <c r="D70" t="s">
         <v>170</v>
-      </c>
-      <c r="D70" t="s">
-        <v>179</v>
       </c>
       <c r="E70" t="s">
         <v>21</v>
@@ -3623,7 +3636,7 @@
         <v>7</v>
       </c>
       <c r="K70" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O70" t="s">
         <v>23</v>
@@ -3635,7 +3648,7 @@
         <v>21</v>
       </c>
       <c r="T70" s="4" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="U70">
         <v>395</v>
@@ -3650,7 +3663,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:24">
+    <row r="71" spans="1:29">
       <c r="A71" t="s">
         <v>18</v>
       </c>
@@ -3658,10 +3671,10 @@
         <v>19</v>
       </c>
       <c r="C71" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D71" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E71" t="s">
         <v>21</v>
@@ -3676,7 +3689,7 @@
         <v>8</v>
       </c>
       <c r="K71" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O71" t="s">
         <v>23</v>
@@ -3688,7 +3701,7 @@
         <v>21</v>
       </c>
       <c r="T71" s="4" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="U71">
         <v>405</v>
@@ -3703,7 +3716,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="72" spans="1:24">
+    <row r="72" spans="1:29">
       <c r="A72" t="s">
         <v>18</v>
       </c>
@@ -3711,10 +3724,10 @@
         <v>19</v>
       </c>
       <c r="C72" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D72" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E72" t="s">
         <v>21</v>
@@ -3729,7 +3742,7 @@
         <v>9</v>
       </c>
       <c r="K72" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O72" t="s">
         <v>23</v>
@@ -3741,7 +3754,7 @@
         <v>21</v>
       </c>
       <c r="T72" s="4" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="U72">
         <v>415</v>
@@ -3756,7 +3769,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="1:24">
+    <row r="73" spans="1:29">
       <c r="A73" t="s">
         <v>18</v>
       </c>
@@ -3767,7 +3780,7 @@
         <v>20</v>
       </c>
       <c r="D73" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E73" t="s">
         <v>21</v>
@@ -3782,7 +3795,7 @@
         <v>10</v>
       </c>
       <c r="K73" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O73" t="s">
         <v>23</v>
@@ -3794,7 +3807,7 @@
         <v>21</v>
       </c>
       <c r="T73" s="4" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="U73">
         <v>425</v>
@@ -3809,7 +3822,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:24">
+    <row r="74" spans="1:29">
       <c r="A74" t="s">
         <v>18</v>
       </c>
@@ -3817,10 +3830,10 @@
         <v>19</v>
       </c>
       <c r="C74" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D74" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E74" t="s">
         <v>21</v>
@@ -3835,7 +3848,7 @@
         <v>11</v>
       </c>
       <c r="K74" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O74" t="s">
         <v>23</v>
@@ -3847,7 +3860,7 @@
         <v>21</v>
       </c>
       <c r="T74" s="4" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="U74">
         <v>435</v>
@@ -3862,7 +3875,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="1:24">
+    <row r="75" spans="1:29">
       <c r="A75" t="s">
         <v>18</v>
       </c>
@@ -3870,10 +3883,10 @@
         <v>19</v>
       </c>
       <c r="C75" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D75" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E75" t="s">
         <v>21</v>
@@ -3888,7 +3901,7 @@
         <v>12</v>
       </c>
       <c r="K75" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O75" t="s">
         <v>23</v>
@@ -3900,7 +3913,7 @@
         <v>21</v>
       </c>
       <c r="T75" s="4" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="U75">
         <v>445</v>
@@ -3915,7 +3928,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:24">
+    <row r="76" spans="1:29">
       <c r="A76" t="s">
         <v>18</v>
       </c>
@@ -3923,10 +3936,10 @@
         <v>19</v>
       </c>
       <c r="C76" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D76" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E76" t="s">
         <v>21</v>
@@ -3941,7 +3954,7 @@
         <v>13</v>
       </c>
       <c r="K76" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O76" t="s">
         <v>23</v>
@@ -3953,7 +3966,7 @@
         <v>21</v>
       </c>
       <c r="T76" s="4" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="U76">
         <v>455</v>
@@ -3968,7 +3981,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:24">
+    <row r="77" spans="1:29">
       <c r="A77" t="s">
         <v>18</v>
       </c>
@@ -3976,10 +3989,10 @@
         <v>19</v>
       </c>
       <c r="C77" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D77" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E77" t="s">
         <v>21</v>
@@ -3994,7 +4007,7 @@
         <v>14</v>
       </c>
       <c r="K77" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O77" t="s">
         <v>23</v>
@@ -4006,7 +4019,7 @@
         <v>21</v>
       </c>
       <c r="T77" s="4" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="U77">
         <v>465</v>
@@ -4021,7 +4034,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="78" spans="1:24">
+    <row r="78" spans="1:29">
       <c r="A78" t="s">
         <v>18</v>
       </c>
@@ -4029,10 +4042,10 @@
         <v>19</v>
       </c>
       <c r="C78" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="D78" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E78" t="s">
         <v>21</v>
@@ -4047,7 +4060,7 @@
         <v>15</v>
       </c>
       <c r="K78" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="O78" t="s">
         <v>23</v>
@@ -4059,7 +4072,7 @@
         <v>21</v>
       </c>
       <c r="T78" s="4" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="U78">
         <v>475</v>
@@ -4072,6 +4085,117 @@
       </c>
       <c r="X78" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="1:29">
+      <c r="A79" t="s">
+        <v>200</v>
+      </c>
+      <c r="B79" t="s">
+        <v>146</v>
+      </c>
+      <c r="R79" t="s">
+        <v>147</v>
+      </c>
+      <c r="T79" t="s">
+        <v>148</v>
+      </c>
+      <c r="U79">
+        <v>5</v>
+      </c>
+      <c r="V79" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y79" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z79" t="s">
+        <v>198</v>
+      </c>
+      <c r="AA79" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB79">
+        <v>2018</v>
+      </c>
+      <c r="AC79" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80" spans="1:29">
+      <c r="A80" t="s">
+        <v>206</v>
+      </c>
+      <c r="B80" t="s">
+        <v>146</v>
+      </c>
+      <c r="R80" t="s">
+        <v>149</v>
+      </c>
+      <c r="T80" t="s">
+        <v>150</v>
+      </c>
+      <c r="U80">
+        <v>4</v>
+      </c>
+      <c r="V80" t="s">
+        <v>26</v>
+      </c>
+      <c r="W80" t="s">
+        <v>151</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>201</v>
+      </c>
+      <c r="Z80" t="s">
+        <v>202</v>
+      </c>
+      <c r="AA80" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB80" s="2">
+        <v>43809</v>
+      </c>
+      <c r="AC80" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="81" spans="1:29">
+      <c r="A81" t="s">
+        <v>205</v>
+      </c>
+      <c r="B81" t="s">
+        <v>146</v>
+      </c>
+      <c r="R81" t="s">
+        <v>149</v>
+      </c>
+      <c r="T81" t="s">
+        <v>152</v>
+      </c>
+      <c r="U81">
+        <v>7</v>
+      </c>
+      <c r="V81" t="s">
+        <v>36</v>
+      </c>
+      <c r="W81" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y81" t="s">
+        <v>204</v>
+      </c>
+      <c r="Z81" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA81" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB81" s="2">
+        <v>43809</v>
+      </c>
+      <c r="AC81" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -4090,8 +4214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5488032-BB51-4744-B401-BCB2F6646798}">
   <dimension ref="A1:AD4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC5" sqref="AC5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1:AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
@@ -4174,36 +4298,36 @@
         <v>17</v>
       </c>
       <c r="Y1" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z1" t="s">
         <v>140</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>141</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>142</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>143</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>144</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:30">
       <c r="A2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+      <c r="R2" t="s">
         <v>147</v>
       </c>
-      <c r="B2" t="s">
-        <v>149</v>
-      </c>
-      <c r="R2" t="s">
-        <v>150</v>
-      </c>
       <c r="T2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="U2">
         <v>5</v>
@@ -4212,13 +4336,13 @@
         <v>36</v>
       </c>
       <c r="Y2" t="s">
-        <v>146</v>
+        <v>199</v>
       </c>
       <c r="Z2" t="s">
-        <v>139</v>
+        <v>198</v>
       </c>
       <c r="AA2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AB2">
         <v>2018</v>
@@ -4229,16 +4353,16 @@
     </row>
     <row r="3" spans="1:30">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s">
+        <v>146</v>
+      </c>
+      <c r="R3" t="s">
         <v>149</v>
       </c>
-      <c r="R3" t="s">
-        <v>154</v>
-      </c>
       <c r="T3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="U3">
         <v>4</v>
@@ -4247,16 +4371,16 @@
         <v>26</v>
       </c>
       <c r="W3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="Y3" t="s">
-        <v>153</v>
+        <v>201</v>
       </c>
       <c r="Z3" t="s">
-        <v>152</v>
+        <v>202</v>
       </c>
       <c r="AA3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AB3" s="2">
         <v>43809</v>
@@ -4267,13 +4391,16 @@
     </row>
     <row r="4" spans="1:30">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>205</v>
+      </c>
+      <c r="B4" t="s">
+        <v>146</v>
       </c>
       <c r="R4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="T4" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="U4">
         <v>7</v>
@@ -4282,16 +4409,16 @@
         <v>36</v>
       </c>
       <c r="W4" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="Y4" t="s">
-        <v>158</v>
+        <v>204</v>
       </c>
       <c r="Z4" t="s">
-        <v>157</v>
+        <v>203</v>
       </c>
       <c r="AA4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="AB4" s="2">
         <v>43809</v>
@@ -4307,46 +4434,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5CA3F7-3463-4F3E-BB07-77B22D87594D}">
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:X16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5"/>
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C1" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="E1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="G1" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H1" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="I1" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:24">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B2">
         <v>68</v>
@@ -4376,7 +4503,7 @@
     </row>
     <row r="3" spans="1:24" hidden="1">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B3">
         <v>116</v>
@@ -4487,7 +4614,7 @@
     </row>
     <row r="7" spans="1:24">
       <c r="A7" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B7">
         <f>B6-B2</f>
@@ -4520,7 +4647,7 @@
     </row>
     <row r="9" spans="1:24">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:24">
@@ -4605,13 +4732,13 @@
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E11" t="s">
         <v>135</v>
       </c>
       <c r="K11" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="N11" t="s">
         <v>26</v>
@@ -4640,7 +4767,7 @@
         <v>69</v>
       </c>
       <c r="K12" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="M12">
         <v>43</v>
@@ -4659,6 +4786,107 @@
       </c>
       <c r="W12">
         <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="A14" t="s">
+        <v>208</v>
+      </c>
+      <c r="B14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" t="s">
+        <v>175</v>
+      </c>
+      <c r="E14" t="s">
+        <v>176</v>
+      </c>
+      <c r="F14" t="s">
+        <v>177</v>
+      </c>
+      <c r="G14" t="s">
+        <v>178</v>
+      </c>
+      <c r="H14" t="s">
+        <v>179</v>
+      </c>
+      <c r="I14" t="s">
+        <v>207</v>
+      </c>
+      <c r="J14" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>71</v>
+      </c>
+      <c r="C15">
+        <v>71</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15">
+        <v>19</v>
+      </c>
+      <c r="F15">
+        <v>45</v>
+      </c>
+      <c r="G15">
+        <v>51</v>
+      </c>
+      <c r="H15">
+        <v>23</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <f>SUM(B15:I15)</f>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>72</v>
+      </c>
+      <c r="C16">
+        <v>72</v>
+      </c>
+      <c r="D16">
+        <v>14</v>
+      </c>
+      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <v>46</v>
+      </c>
+      <c r="G16">
+        <v>52</v>
+      </c>
+      <c r="H16">
+        <v>23</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <f>SUM(B16:I16)</f>
+        <v>302</v>
+      </c>
+      <c r="K16" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>